<commit_message>
Deploy updated output folder
</commit_message>
<xml_diff>
--- a/CodeSystem-nigeria-facility-type.xlsx
+++ b/CodeSystem-nigeria-facility-type.xlsx
@@ -57,19 +57,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-31T19:23:08+01:00</t>
+    <t>2025-08-02T14:19:18+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>https://dhin-hie.org</t>
+    <t>https://www.dhin-hie.org</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>https://dhin-hie.org (https://dhin-hie.org, info@dhin-hie.org)</t>
+    <t>https://www.dhin-hie.org (https://www.dhin-hie.org/IGs, info@dhin-hie.org)</t>
   </si>
   <si>
     <t>Digital Health Interoperability Network (DHIN). (info@dhin-hie.org(Work))</t>

</xml_diff>